<commit_message>
Correct BOM and add Fusion 360
Corrected a BOM description for one of the extrusions, and added a
Fusion 360 version in the Other 3D Format folder.
</commit_message>
<xml_diff>
--- a/Documentation/BOM/Eustathios Spider V2 BOM.xlsx
+++ b/Documentation/BOM/Eustathios Spider V2 BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25500" windowHeight="13095" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25500" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="SUBASSY" sheetId="1" r:id="rId1"/>
@@ -1279,9 +1279,6 @@
     <t>20x20x562mm Extruded Aluminum W/ Holes</t>
   </si>
   <si>
-    <t>20x20x462mm Extruded Aluminum W/ Tapped Ends</t>
-  </si>
-  <si>
     <t>20x20x321mm Extruded Aluminum W/ Tapped Ends</t>
   </si>
   <si>
@@ -1376,6 +1373,9 @@
   </si>
   <si>
     <t>8mm_Shaft_Hobb_Gear</t>
+  </si>
+  <si>
+    <t>20x20x425mm Extruded Aluminum W/ Tapped Ends</t>
   </si>
 </sst>
 </file>
@@ -7492,9 +7492,9 @@
   </sheetPr>
   <dimension ref="A1:H275"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7583,7 +7583,7 @@
         <v>142</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>412</v>
+        <v>444</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>394</v>
@@ -10201,7 +10201,7 @@
         <v>78</v>
       </c>
       <c r="D121" s="125" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E121" s="20" t="s">
         <v>394</v>
@@ -10638,7 +10638,7 @@
         <v>182</v>
       </c>
       <c r="D141" s="117" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E141" s="118" t="s">
         <v>394</v>
@@ -11020,10 +11020,10 @@
         <v>92</v>
       </c>
       <c r="C158" s="28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D158" s="70" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>231</v>
@@ -11046,7 +11046,7 @@
         <v>188</v>
       </c>
       <c r="D159" s="70" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E159" s="9" t="s">
         <v>231</v>
@@ -11138,10 +11138,10 @@
         <v>265</v>
       </c>
       <c r="D163" s="62" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E163" s="63" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F163" s="63"/>
       <c r="G163" s="63">
@@ -11181,13 +11181,13 @@
         <v>10.8</v>
       </c>
       <c r="C165" s="61" t="s">
+        <v>417</v>
+      </c>
+      <c r="D165" s="62" t="s">
         <v>418</v>
       </c>
-      <c r="D165" s="62" t="s">
+      <c r="E165" s="63" t="s">
         <v>419</v>
-      </c>
-      <c r="E165" s="63" t="s">
-        <v>420</v>
       </c>
       <c r="F165" s="63"/>
       <c r="G165" s="63">
@@ -11210,7 +11210,7 @@
         <v>316</v>
       </c>
       <c r="E166" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F166" s="9"/>
       <c r="G166" s="9">
@@ -11230,7 +11230,7 @@
         <v>191</v>
       </c>
       <c r="D167" s="62" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E167" s="63" t="s">
         <v>392</v>
@@ -11250,7 +11250,7 @@
         <v>192</v>
       </c>
       <c r="D168" s="85" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E168" s="63" t="s">
         <v>394</v>
@@ -11474,7 +11474,7 @@
         <v>106</v>
       </c>
       <c r="C178" s="70" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D178" s="70" t="s">
         <v>388</v>
@@ -11500,7 +11500,7 @@
         <v>322</v>
       </c>
       <c r="D179" s="70" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E179" s="9" t="s">
         <v>390</v>
@@ -11592,7 +11592,7 @@
         <v>196</v>
       </c>
       <c r="D183" s="70" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E183" s="9" t="s">
         <v>231</v>
@@ -11750,7 +11750,7 @@
         <v>322</v>
       </c>
       <c r="D190" s="85" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E190" s="63" t="s">
         <v>390</v>
@@ -11842,7 +11842,7 @@
         <v>196</v>
       </c>
       <c r="D194" s="85" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E194" s="63" t="s">
         <v>231</v>
@@ -11934,7 +11934,7 @@
         <v>198</v>
       </c>
       <c r="E198" s="63" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F198" s="63"/>
       <c r="G198" s="63">
@@ -11957,7 +11957,7 @@
         <v>199</v>
       </c>
       <c r="E199" s="63" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F199" s="63"/>
       <c r="G199" s="63">
@@ -11980,7 +11980,7 @@
         <v>200</v>
       </c>
       <c r="E200" s="63" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F200" s="63"/>
       <c r="G200" s="63">
@@ -12003,7 +12003,7 @@
         <v>201</v>
       </c>
       <c r="E201" s="63" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F201" s="63"/>
       <c r="G201" s="63">
@@ -12020,10 +12020,10 @@
         <v>129</v>
       </c>
       <c r="C202" s="84" t="s">
+        <v>428</v>
+      </c>
+      <c r="D202" s="84" t="s">
         <v>429</v>
-      </c>
-      <c r="D202" s="84" t="s">
-        <v>430</v>
       </c>
       <c r="E202" s="63" t="s">
         <v>231</v>
@@ -12049,7 +12049,7 @@
         <v>202</v>
       </c>
       <c r="E203" s="63" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F203" s="99"/>
       <c r="G203" s="99">
@@ -12331,7 +12331,7 @@
         <v>361</v>
       </c>
       <c r="D216" s="62" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E216" s="63" t="s">
         <v>395</v>
@@ -12416,7 +12416,7 @@
         <v>361</v>
       </c>
       <c r="D220" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E220" s="9" t="s">
         <v>395</v>
@@ -12559,7 +12559,7 @@
         <v>338</v>
       </c>
       <c r="E226" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F226" s="67"/>
       <c r="G226" s="67"/>
@@ -12640,7 +12640,7 @@
         <v>342</v>
       </c>
       <c r="E230" s="63" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F230" s="63"/>
       <c r="G230" s="63">
@@ -12879,7 +12879,7 @@
         <v>353</v>
       </c>
       <c r="E241" s="63" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F241" s="63"/>
       <c r="G241" s="63">
@@ -13137,13 +13137,13 @@
         <v>20.5</v>
       </c>
       <c r="C253" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D253" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="E253" s="9" t="s">
         <v>434</v>
-      </c>
-      <c r="E253" s="9" t="s">
-        <v>435</v>
       </c>
       <c r="F253" s="9"/>
       <c r="G253" s="9">
@@ -13163,7 +13163,7 @@
         <v>374</v>
       </c>
       <c r="D254" s="62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E254" s="63" t="s">
         <v>390</v>
@@ -13499,10 +13499,10 @@
         <v>358</v>
       </c>
       <c r="C269" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D269" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E269" s="9" t="s">
         <v>390</v>
@@ -13672,7 +13672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -13684,10 +13684,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="137" t="s">
+        <v>440</v>
+      </c>
+      <c r="B1" s="138" t="s">
         <v>441</v>
-      </c>
-      <c r="B1" s="138" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -13940,7 +13940,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="135" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B33" s="136">
         <v>1</v>
@@ -13948,7 +13948,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="134" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B34" s="108">
         <v>1</v>
@@ -13956,7 +13956,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="135" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B35" s="136">
         <v>1</v>
@@ -14084,7 +14084,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="135" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B51" s="136">
         <v>1</v>
@@ -14148,7 +14148,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="135" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B59" s="136">
         <v>1</v>
@@ -14156,7 +14156,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="134" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B60" s="108">
         <v>1</v>
@@ -14188,7 +14188,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="134" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B64" s="108">
         <v>1</v>
@@ -14356,7 +14356,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="134" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B85" s="108">
         <v>1</v>
@@ -14428,7 +14428,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="134" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B94" s="108">
         <v>4</v>
@@ -14572,7 +14572,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="135" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B112" s="136">
         <v>2</v>
@@ -14604,7 +14604,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="134" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B116" s="108">
         <v>1</v>
@@ -14724,7 +14724,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="135" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B131" s="136">
         <v>6</v>
@@ -14812,7 +14812,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="135" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B142" s="136">
         <v>1</v>
@@ -14828,13 +14828,13 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="141" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B144" s="142"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="133" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B145" s="108">
         <v>597</v>

</xml_diff>